<commit_message>
fix 27/4/2024 lần 1
</commit_message>
<xml_diff>
--- a/shoeStoreAPI/src/main/resources/reports/BaoCaoBanHang.xlsx
+++ b/shoeStoreAPI/src/main/resources/reports/BaoCaoBanHang.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FITHOU\DATN\Code\quanghungglasses-api\src\main\resources\static\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DoAnTotNghiep\project\shoeStoreAPI\src\main\resources\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34114CEA-F5A9-497F-919F-E81B87236DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A5AC66-8B4E-4EA8-A2BD-0AEA696224EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tháng 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="13">
   <si>
     <t>Mã SP</t>
   </si>
@@ -57,13 +57,31 @@
   </si>
   <si>
     <t>STT</t>
+  </si>
+  <si>
+    <t>Mã sản phẩm</t>
+  </si>
+  <si>
+    <t>Tên sản phẩm</t>
+  </si>
+  <si>
+    <t>Màu sắc</t>
+  </si>
+  <si>
+    <t>Kích cỡ</t>
+  </si>
+  <si>
+    <t>Thành tiền</t>
+  </si>
+  <si>
+    <t>Số lượng bán</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +109,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -100,7 +125,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -123,16 +148,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -418,49 +462,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" style="1"/>
-    <col min="3" max="3" width="26.7109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="1"/>
-    <col min="6" max="6" width="19.28515625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="22.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="42.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>4</v>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -479,26 +529,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" style="1"/>
-    <col min="3" max="3" width="26.7109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="1"/>
-    <col min="6" max="6" width="19.28515625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="19.33203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -534,26 +584,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" style="1"/>
-    <col min="3" max="3" width="26.7109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="1"/>
-    <col min="6" max="6" width="19.28515625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="19.33203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -589,26 +639,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" style="1"/>
-    <col min="3" max="3" width="26.7109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="1"/>
-    <col min="6" max="6" width="19.28515625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="19.33203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -644,26 +694,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" style="1"/>
-    <col min="3" max="3" width="26.7109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="1"/>
-    <col min="6" max="6" width="19.28515625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="19.33203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -699,26 +749,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" style="1"/>
-    <col min="3" max="3" width="26.7109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="1"/>
-    <col min="6" max="6" width="19.28515625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="19.33203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -754,26 +804,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" style="1"/>
-    <col min="3" max="3" width="26.7109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="1"/>
-    <col min="6" max="6" width="19.28515625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="19.33203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -809,26 +859,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" style="1"/>
-    <col min="3" max="3" width="26.7109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="1"/>
-    <col min="6" max="6" width="19.28515625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="19.33203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -864,26 +914,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" style="1"/>
-    <col min="3" max="3" width="26.7109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="1"/>
-    <col min="6" max="6" width="19.28515625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="19.33203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -919,26 +969,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" style="1"/>
-    <col min="3" max="3" width="26.7109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="1"/>
-    <col min="6" max="6" width="19.28515625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="19.33203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -974,26 +1024,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" style="1"/>
-    <col min="3" max="3" width="26.7109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="1"/>
-    <col min="6" max="6" width="19.28515625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="19.33203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1029,26 +1079,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" style="1"/>
-    <col min="3" max="3" width="26.7109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="1"/>
-    <col min="6" max="6" width="19.28515625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="19.33203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>

</xml_diff>